<commit_message>
mostrando o risco do trade no frontend ao fazer trade
</commit_message>
<xml_diff>
--- a/docs/CalculoRisco.xlsx
+++ b/docs/CalculoRisco.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>ValorCompra</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>PercRiscoAtual</t>
+  </si>
+  <si>
+    <t>RiscoAtual</t>
   </si>
 </sst>
 </file>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:N27"/>
+  <dimension ref="A4:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +576,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>64800</v>
+      </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -617,12 +623,18 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6*B12</f>
+        <v>3888</v>
+      </c>
+    </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8">
-        <f>B23</f>
+        <f>B24</f>
         <v>20</v>
       </c>
       <c r="E8">
@@ -644,7 +656,7 @@
         <v>-1500</v>
       </c>
       <c r="J8">
-        <f>B24</f>
+        <f>B25</f>
         <v>18</v>
       </c>
       <c r="K8">
@@ -759,58 +771,67 @@
         <v>730</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <f>B15*B14</f>
+        <v>1035.6164383561643</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <f>B23-B24</f>
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B25">
-        <f>B20/$C$24</f>
-        <v>365</v>
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <f>B24-B25</f>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <f>B17/$C$24</f>
-        <v>595</v>
+        <f>B20/$C$25</f>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <f>B17/$C$25</f>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
-      <c r="B27">
-        <f>SMALL(B25:B26,1)</f>
+      <c r="B28">
+        <f>SMALL(B26:B27,1)</f>
         <v>365</v>
       </c>
     </row>

</xml_diff>